<commit_message>
psa_water_sensor install and uninstall
updated wording around manually typing of barcodes for nodes and gateways
</commit_message>
<xml_diff>
--- a/forms/psa_water_sensor_install/psa_water_sensor_install.xlsx
+++ b/forms/psa_water_sensor_install/psa_water_sensor_install.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="120">
   <si>
     <t>type</t>
   </si>
@@ -296,9 +296,6 @@
     <t>Barcode didn't scan?</t>
   </si>
   <si>
-    <t>Try again. If it fails multiple times you can manually type the barcode here. IMPORTANT: Double check and use correct cases and dashes.</t>
-  </si>
-  <si>
     <t>fail000</t>
   </si>
   <si>
@@ -383,7 +380,7 @@
     <t>alt_bare_node_rep2</t>
   </si>
   <si>
-    <t>IMPORTANT: Double check correct numbers</t>
+    <t>Manually type here. IMPORTANT: Double check correct numbers</t>
   </si>
 </sst>
 </file>
@@ -735,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -960,10 +957,10 @@
         <v>30</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -973,7 +970,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -1051,10 +1048,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>90</v>
@@ -1073,10 +1070,10 @@
         <v>30</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1086,7 +1083,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -1119,10 +1116,10 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>90</v>
@@ -1141,10 +1138,10 @@
         <v>30</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -1154,7 +1151,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
@@ -1215,10 +1212,10 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>90</v>
@@ -1237,10 +1234,10 @@
         <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1250,7 +1247,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
@@ -1283,10 +1280,10 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>90</v>
@@ -1305,10 +1302,10 @@
         <v>30</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -1318,7 +1315,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
@@ -1447,57 +1444,57 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Water sensor install V5
added winter testing option
if it is winter or re-installation, users won't be prompted to add crop planting date.
removed crop all together
</commit_message>
<xml_diff>
--- a/forms/psa_water_sensor_install/psa_water_sensor_install.xlsx
+++ b/forms/psa_water_sensor_install/psa_water_sensor_install.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="128">
   <si>
     <t>type</t>
   </si>
@@ -98,18 +98,12 @@
     <t>sensorplacerep1</t>
   </si>
   <si>
-    <t>Sensorplacerep1.jpg</t>
-  </si>
-  <si>
     <t>sensorplacerep2</t>
   </si>
   <si>
     <t>In the second rep, you will not have a surface sensor</t>
   </si>
   <si>
-    <t>Sensorplacerep2.jpg</t>
-  </si>
-  <si>
     <t>text</t>
   </si>
   <si>
@@ -395,16 +389,22 @@
     <t>What is the date the crop was planted?</t>
   </si>
   <si>
-    <t>crop</t>
-  </si>
-  <si>
-    <t>What is the crop?</t>
-  </si>
-  <si>
-    <t>v4</t>
-  </si>
-  <si>
     <t>${initial_or_reinstall}='re-install'</t>
+  </si>
+  <si>
+    <t>Winter Install</t>
+  </si>
+  <si>
+    <t>winter</t>
+  </si>
+  <si>
+    <t>v5</t>
+  </si>
+  <si>
+    <t>bagandsensorplacementrep1.jpg</t>
+  </si>
+  <si>
+    <t>bagandsensorplacementrep2.jpg</t>
   </si>
 </sst>
 </file>
@@ -762,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -774,7 +774,7 @@
     <col min="2" max="2" width="32.453125" customWidth="1"/>
     <col min="3" max="3" width="43.08984375" customWidth="1"/>
     <col min="4" max="4" width="16.1796875" customWidth="1"/>
-    <col min="7" max="7" width="5.453125" customWidth="1"/>
+    <col min="7" max="7" width="28.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.36328125" customWidth="1"/>
     <col min="9" max="9" width="16.90625" customWidth="1"/>
   </cols>
@@ -805,7 +805,7 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -826,18 +826,18 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -882,7 +882,7 @@
         <v>20</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F8" t="s">
         <v>18</v>
@@ -915,13 +915,13 @@
         <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F11" t="s">
         <v>18</v>
       </c>
       <c r="G11" t="s">
-        <v>25</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -929,16 +929,16 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
         <v>26</v>
       </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
       <c r="F12" t="s">
         <v>18</v>
       </c>
       <c r="G12" t="s">
-        <v>28</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -946,7 +946,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D13" t="s">
         <v>13</v>
@@ -954,27 +954,27 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B14" t="s">
+      <c r="F14" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
         <v>36</v>
-      </c>
-      <c r="B15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" t="s">
-        <v>38</v>
       </c>
       <c r="F15" t="s">
         <v>18</v>
@@ -985,94 +985,96 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" t="s">
         <v>77</v>
-      </c>
-      <c r="C16" t="s">
-        <v>79</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F17" t="b">
         <v>0</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>123</v>
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>68</v>
       </c>
       <c r="F18" t="b">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>121</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" t="s">
-        <v>70</v>
-      </c>
-      <c r="F19" t="b">
-        <v>1</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>31</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" t="b">
-        <v>1</v>
-      </c>
+      <c r="A21" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1081,83 +1083,83 @@
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2" t="s">
-        <v>102</v>
-      </c>
+      <c r="I22" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="I26" s="1"/>
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="C27" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
+        <v>63</v>
+      </c>
+      <c r="F28" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" t="s">
-        <v>65</v>
-      </c>
-      <c r="F29" t="s">
-        <v>18</v>
-      </c>
+      <c r="A29" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>110</v>
+        <v>27</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1166,66 +1168,66 @@
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
+      <c r="I30" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2" t="s">
-        <v>112</v>
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" t="s">
+        <v>80</v>
+      </c>
+      <c r="F31" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C32" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="F32" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" t="s">
-        <v>61</v>
-      </c>
-      <c r="C33" t="s">
-        <v>68</v>
-      </c>
-      <c r="F33" t="s">
-        <v>18</v>
-      </c>
+      <c r="A33" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
-        <v>109</v>
+        <v>27</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -1234,38 +1236,33 @@
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
+      <c r="I34" s="2" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2" t="s">
-        <v>113</v>
+      <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" t="s">
+        <v>81</v>
+      </c>
+      <c r="F35" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B36" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="C36" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F36" t="s">
         <v>18</v>
@@ -1273,13 +1270,13 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C37" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="F37" t="s">
         <v>18</v>
@@ -1287,41 +1284,46 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B38" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="C38" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F38" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>33</v>
-      </c>
-      <c r="B39" t="s">
-        <v>57</v>
-      </c>
-      <c r="C39" t="s">
-        <v>66</v>
-      </c>
-      <c r="F39" t="s">
-        <v>18</v>
-      </c>
+      <c r="A39" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
-        <v>108</v>
+        <v>27</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -1330,66 +1332,66 @@
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
+      <c r="I40" s="2" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A41" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2" t="s">
-        <v>114</v>
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" t="s">
+        <v>78</v>
+      </c>
+      <c r="F41" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B42" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C42" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="F42" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>33</v>
-      </c>
-      <c r="B43" t="s">
-        <v>58</v>
-      </c>
-      <c r="C43" t="s">
-        <v>67</v>
-      </c>
-      <c r="F43" t="s">
-        <v>18</v>
-      </c>
+      <c r="A43" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
-        <v>107</v>
+        <v>27</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -1398,38 +1400,33 @@
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
+      <c r="I44" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A45" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2" t="s">
-        <v>115</v>
+      <c r="A45" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" t="s">
+        <v>79</v>
+      </c>
+      <c r="F45" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B46" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="C46" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F46" t="s">
         <v>18</v>
@@ -1437,13 +1434,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>29</v>
-      </c>
-      <c r="B47" t="s">
-        <v>73</v>
-      </c>
-      <c r="C47" t="s">
-        <v>85</v>
+        <v>23</v>
       </c>
       <c r="F47" t="s">
         <v>18</v>
@@ -1451,23 +1442,15 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>23</v>
+        <v>14</v>
+      </c>
+      <c r="B48" t="s">
+        <v>42</v>
+      </c>
+      <c r="C48" t="s">
+        <v>43</v>
       </c>
       <c r="F48" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>14</v>
-      </c>
-      <c r="B49" t="s">
-        <v>44</v>
-      </c>
-      <c r="C49" t="s">
-        <v>45</v>
-      </c>
-      <c r="F49" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1479,10 +1462,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1493,7 +1476,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1504,105 +1487,117 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
         <v>47</v>
-      </c>
-      <c r="B2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" t="s">
-        <v>54</v>
+      <c r="A4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
         <v>52</v>
-      </c>
-      <c r="B5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>101</v>
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>90</v>
-      </c>
-      <c r="B7" t="s">
-        <v>98</v>
+        <v>87</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="C7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" t="s">
         <v>93</v>
       </c>
-      <c r="B10" t="s">
-        <v>116</v>
-      </c>
-      <c r="C10" t="s">
-        <v>96</v>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>